<commit_message>
Setup: initial repo template for kick-off
</commit_message>
<xml_diff>
--- a/docs/reparto tareas.xlsx
+++ b/docs/reparto tareas.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Backend &amp; datos" sheetId="1" state="visible" r:id="rId3"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
   <si>
     <t xml:space="preserve">Módulo/Tarea</t>
   </si>
@@ -88,6 +88,81 @@
   </si>
   <si>
     <t xml:space="preserve">Implementar las funciones de backend para anonimizar o eliminar datos cuando un usuario lo solicite.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A. Selección del Algoritmo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No se deben utilizar funciones de hash rápidas (como MD5 o SHA-1). Se deben implementar algoritmos diseñados específicamente para el almacenamiento de contraseñas que incluyan un "factor de trabajo" (work factor) ajustable:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recomendados: Argon2 (ganador del Password Hashing Competition), BCrypt o SCrypt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B. Implementación de "Sal" (Salting)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generación de una cadena aleatoria única para cada usuario que se combina con la contraseña antes del hasheo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Función: Evita que dos usuarios con la misma contraseña tengan el mismo hash y neutraliza el uso de Rainbow Tables (tablas de hashes precalculados).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C. Lógica de Verificación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desarrollar el flujo de autenticación donde:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se recibe la contraseña en texto plano durante el Login.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se recupera el hash y la sal almacenados para ese usuario.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se aplica el mismo proceso de hasheo a la contraseña recibida.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se comparan los resultados mediante una comparación de tiempo constante para evitar ataques de canal lateral (timing attacks).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Flujo de Trabajo (Workflow)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acción</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proceso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resultado en BD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contraseña + Salt → Algoritmo (Argon2/BCrypt)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Almacena Salt y Hash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contraseña ingresada + Salt recuperada → Algoritmo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comparación con Hash guardado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cambio Clave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nueva Contraseña + Nueva Salt → Algoritmo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actualiza Salt y Hash</t>
   </si>
   <si>
     <t xml:space="preserve">Implement a complete web-based game</t>
@@ -325,7 +400,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,6 +435,14 @@
       <sz val="11"/>
       <color rgb="FF1F1F1F"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -434,21 +517,37 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -511,7 +610,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF00A933"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF1F1F1F"/>
       <rgbColor rgb="FF993300"/>
@@ -698,85 +797,198 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
+    <tabColor rgb="FF00A933"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="52.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="52.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -797,69 +1009,69 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="38.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
+      <c r="C2" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
+      <c r="C3" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>20</v>
+      <c r="C4" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>22</v>
+      <c r="C5" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -876,73 +1088,74 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
+    <tabColor rgb="FF00A933"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="44.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
+      <c r="C2" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>25</v>
+      <c r="C3" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>27</v>
+      <c r="C4" s="4" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>30</v>
+      <c r="A5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -959,74 +1172,75 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
+    <tabColor rgb="FF00A933"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="42.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="42.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="52.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>32</v>
+      <c r="C2" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>35</v>
+      <c r="A3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>37</v>
+      <c r="A4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>40</v>
+      <c r="A5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>